<commit_message>
Since we send two images, we need twice the number of tokens
</commit_message>
<xml_diff>
--- a/docs/CostAnalysis.xlsx
+++ b/docs/CostAnalysis.xlsx
@@ -152,19 +152,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
     <numFmt numFmtId="166" formatCode="#,##0.00"/>
     <numFmt numFmtId="167" formatCode="@"/>
-    <numFmt numFmtId="168" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
-    <numFmt numFmtId="169" formatCode="General"/>
   </numFmts>
   <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -185,12 +184,14 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -235,60 +236,68 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -418,379 +427,379 @@
   <dimension ref="C4:I40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C39" activeCellId="0" sqref="C39:H40"/>
+      <selection pane="topLeft" activeCell="E40" activeCellId="0" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="30.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="38.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="36.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="37.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="30.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="38.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="36.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="37.69"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="3" t="n">
+      <c r="D6" s="4" t="n">
         <v>0.4</v>
       </c>
-      <c r="E6" s="3" t="n">
+      <c r="E6" s="4" t="n">
         <v>0.4</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="6" t="n">
+      <c r="I6" s="7" t="n">
         <v>8.344</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="3" t="n">
+      <c r="D7" s="4" t="n">
         <v>1.6</v>
       </c>
-      <c r="E7" s="3" t="n">
+      <c r="E7" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="8" t="n">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="9" t="n">
         <f aca="false">SUM(F6,F7)</f>
         <v>0</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="5" t="s">
+      <c r="G8" s="3"/>
+      <c r="H8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10" t="s">
+      <c r="E14" s="11"/>
+      <c r="F14" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="10"/>
+      <c r="G14" s="11"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="0" t="s">
+      <c r="F15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="0" t="s">
+      <c r="G15" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="1" t="n">
         <f aca="false">H6*24*365</f>
         <v>56852.4</v>
       </c>
-      <c r="E16" s="11" t="n">
+      <c r="E16" s="12" t="n">
         <f aca="false">I6*24*365</f>
         <v>73093.44</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D17" s="1" t="n">
         <f aca="false">D16/12</f>
         <v>4737.7</v>
       </c>
-      <c r="E17" s="11" t="n">
+      <c r="E17" s="12" t="n">
         <f aca="false">E16/12</f>
         <v>6091.12</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D22" s="0" t="s">
+      <c r="D22" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E22" s="0" t="s">
+      <c r="E22" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="9" t="n">
+      <c r="D23" s="10" t="n">
         <v>2048</v>
       </c>
-      <c r="E23" s="0" t="n">
+      <c r="E23" s="1" t="n">
         <v>1536</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="0" t="s">
+      <c r="C24" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="0" t="n">
+      <c r="D24" s="1" t="n">
         <v>1100</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="0" t="s">
+      <c r="C25" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="0" t="n">
+      <c r="D25" s="1" t="n">
         <v>1600</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="0" t="s">
+      <c r="C26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="0" t="n">
+      <c r="D26" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="E26" s="0" t="n">
+      <c r="E26" s="1" t="n">
         <v>32</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="0" t="s">
+      <c r="C27" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="0" t="n">
+      <c r="D27" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="E27" s="0" t="n">
+      <c r="E27" s="1" t="n">
         <v>32</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="0" t="s">
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G34" s="0" t="s">
+      <c r="G34" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H34" s="0" t="s">
+      <c r="H34" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="12" t="s">
+      <c r="C35" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D35" s="0" t="s">
+      <c r="D35" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E35" s="0" t="n">
-        <f aca="false">(D23/D26*E23/E26) +2 +D24</f>
-        <v>4174</v>
-      </c>
-      <c r="F35" s="13" t="n">
+      <c r="E35" s="1" t="n">
+        <f aca="false">((D23/D26*E23/E26) +2 +D24)*2</f>
+        <v>8348</v>
+      </c>
+      <c r="F35" s="1" t="n">
         <f aca="false">(1000*E35)/1000000*G6</f>
-        <v>12.522</v>
-      </c>
-      <c r="G35" s="12" t="n">
+        <v>25.044</v>
+      </c>
+      <c r="G35" s="13" t="n">
         <f aca="false">SUM(F35:F36)</f>
-        <v>18.522</v>
-      </c>
-      <c r="H35" s="12" t="n">
+        <v>31.044</v>
+      </c>
+      <c r="H35" s="13" t="n">
         <f aca="false">G35*10</f>
-        <v>185.22</v>
+        <v>310.44</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="12"/>
-      <c r="D36" s="0" t="s">
+      <c r="C36" s="13"/>
+      <c r="D36" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E36" s="0" t="n">
+      <c r="E36" s="1" t="n">
         <v>400</v>
       </c>
-      <c r="F36" s="13" t="n">
+      <c r="F36" s="1" t="n">
         <f aca="false">E36*1000/1000000*G7</f>
         <v>6</v>
       </c>
-      <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="12" t="s">
+      <c r="C37" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D37" s="0" t="s">
+      <c r="D37" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E37" s="9" t="n">
-        <f aca="false">(D23/D27*E23/E27)+2+D25</f>
-        <v>4674</v>
-      </c>
-      <c r="F37" s="13" t="n">
+      <c r="E37" s="10" t="n">
+        <f aca="false">2*((D23/D27*E23/E27)+2+D25)</f>
+        <v>9348</v>
+      </c>
+      <c r="F37" s="1" t="n">
         <f aca="false">E37*1000/1000000*F6</f>
-        <v>0.74784</v>
-      </c>
-      <c r="G37" s="12" t="n">
+        <v>1.49568</v>
+      </c>
+      <c r="G37" s="13" t="n">
         <f aca="false">SUM(F37:F38)</f>
-        <v>1.14144</v>
-      </c>
-      <c r="H37" s="12" t="n">
+        <v>1.88928</v>
+      </c>
+      <c r="H37" s="13" t="n">
         <f aca="false">G37*10</f>
-        <v>11.4144</v>
+        <v>18.8928</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C38" s="12"/>
-      <c r="D38" s="0" t="s">
+      <c r="C38" s="13"/>
+      <c r="D38" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E38" s="0" t="n">
+      <c r="E38" s="1" t="n">
         <v>615</v>
       </c>
-      <c r="F38" s="13" t="n">
+      <c r="F38" s="1" t="n">
         <f aca="false">E38*1000/1000000*F7</f>
         <v>0.3936</v>
       </c>
-      <c r="G38" s="12"/>
-      <c r="H38" s="12"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D39" s="0" t="s">
+      <c r="D39" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E39" s="9" t="n">
-        <f aca="false">(D23/D27*E23/E27)+2+D25</f>
-        <v>4674</v>
-      </c>
-      <c r="F39" s="11" t="n">
+      <c r="E39" s="10" t="n">
+        <f aca="false">2*((D23/D27*E23/E27)+2+D25)</f>
+        <v>9348</v>
+      </c>
+      <c r="F39" s="12" t="n">
         <f aca="false">E39*1000/1000000*D6</f>
-        <v>1.8696</v>
-      </c>
-      <c r="G39" s="11" t="n">
+        <v>3.7392</v>
+      </c>
+      <c r="G39" s="15" t="n">
         <f aca="false">SUM(F39:F40)</f>
-        <v>2.8536</v>
-      </c>
-      <c r="H39" s="11" t="n">
+        <v>4.7232</v>
+      </c>
+      <c r="H39" s="15" t="n">
         <f aca="false">G39*10</f>
-        <v>28.536</v>
+        <v>47.232</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C40" s="2"/>
-      <c r="D40" s="0" t="s">
+      <c r="C40" s="14"/>
+      <c r="D40" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E40" s="0" t="n">
+      <c r="E40" s="1" t="n">
         <v>615</v>
       </c>
-      <c r="F40" s="11" t="n">
+      <c r="F40" s="12" t="n">
         <f aca="false">E40*1000/1000000*D7</f>
         <v>0.984</v>
       </c>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="14">

</xml_diff>